<commit_message>
added admin column to users
also unimportant changes in csvs
</commit_message>
<xml_diff>
--- a/data/xlsx/users.xlsx
+++ b/data/xlsx/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>profile_picture</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
   <si>
     <t>created_at</t>
@@ -322,6 +325,9 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>